<commit_message>
Login Using DataDriven Completed
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\japan_office\feb\framework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF537575-599F-4C12-93C9-2D587CA8789E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19B8EA0-B3A8-4858-A811-7E83451C9B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="0" windowWidth="14415" windowHeight="15600" xr2:uid="{E2B93ED8-0A7A-4491-B70A-ED7512AA6DF5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E2B93ED8-0A7A-4491-B70A-ED7512AA6DF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -51,28 +51,13 @@
     <t>locked_out_user</t>
   </si>
   <si>
-    <t>problem_user</t>
-  </si>
-  <si>
-    <t>performance_glitch_user</t>
-  </si>
-  <si>
-    <t>error_user</t>
-  </si>
-  <si>
-    <t>visual_user</t>
-  </si>
-  <si>
     <t>secret_sauce</t>
   </si>
   <si>
-    <t>secretsauce</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>fail</t>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -434,7 +419,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D1" sqref="D1:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,10 +445,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -471,57 +456,30 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>